<commit_message>
Added ERRATA for v2.0, added real values to FTDI oscilator
</commit_message>
<xml_diff>
--- a/docs/BOM.xlsx
+++ b/docs/BOM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21601"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\johnc\Documents\Proyectos\Arriquitaun2.0\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9D8CDE6-3857-4E8A-88BB-88C9FDE7719A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{305C6C5E-004B-4AE8-9D51-A680B290B86C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="396" yWindow="300" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="114">
   <si>
     <t>link</t>
   </si>
@@ -367,6 +367,12 @@
   </si>
   <si>
     <t>523-L77HDE15SD1CH4R</t>
+  </si>
+  <si>
+    <t>Llegado</t>
+  </si>
+  <si>
+    <t>¡!</t>
   </si>
 </sst>
 </file>
@@ -431,7 +437,7 @@
       <family val="1"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -447,6 +453,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -479,7 +491,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -522,6 +534,12 @@
     </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -804,11 +822,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O27"/>
+  <dimension ref="A1:P27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A10" sqref="A10:N10"/>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L25" sqref="L25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="30.6640625" defaultRowHeight="36" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -822,14 +840,15 @@
     <col min="8" max="8" width="9" style="2" bestFit="1" customWidth="1"/>
     <col min="9" max="10" width="9.33203125" style="2" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="10.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.77734375" style="2" customWidth="1"/>
-    <col min="13" max="13" width="15.77734375" style="2" customWidth="1"/>
-    <col min="14" max="14" width="49.88671875" style="2" customWidth="1"/>
-    <col min="15" max="15" width="255.6640625" style="3" customWidth="1"/>
-    <col min="16" max="16384" width="30.6640625" style="2"/>
+    <col min="12" max="12" width="10.33203125" style="2" customWidth="1"/>
+    <col min="13" max="13" width="13.77734375" style="2" customWidth="1"/>
+    <col min="14" max="14" width="15.77734375" style="2" customWidth="1"/>
+    <col min="15" max="15" width="49.88671875" style="2" customWidth="1"/>
+    <col min="16" max="16" width="255.6640625" style="3" customWidth="1"/>
+    <col min="17" max="16384" width="30.6640625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="36" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
         <v>77</v>
       </c>
@@ -863,20 +882,23 @@
       <c r="K1" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L1" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="M1" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="M1" s="6" t="s">
+      <c r="N1" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="O1" s="6" t="s">
+      <c r="P1" s="6" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="36" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:16" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
         <v>3</v>
       </c>
@@ -903,21 +925,24 @@
       <c r="I2" s="8"/>
       <c r="J2" s="8"/>
       <c r="K2" s="8"/>
-      <c r="L2" s="11">
+      <c r="L2" s="15">
+        <v>4</v>
+      </c>
+      <c r="M2" s="11">
         <f>E2*F2</f>
         <v>17.52</v>
       </c>
-      <c r="M2" s="9" t="s">
-        <v>85</v>
-      </c>
-      <c r="N2" s="11" t="s">
+      <c r="N2" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="O2" s="11" t="s">
         <v>86</v>
       </c>
-      <c r="O2" s="13" t="s">
+      <c r="P2" s="13" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:15" ht="36" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:16" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
         <v>4</v>
       </c>
@@ -944,21 +969,24 @@
       <c r="I3" s="8"/>
       <c r="J3" s="8"/>
       <c r="K3" s="8"/>
-      <c r="L3" s="11">
-        <f t="shared" ref="L3:L17" si="1">E3*F3</f>
+      <c r="L3" s="15">
+        <v>4</v>
+      </c>
+      <c r="M3" s="11">
+        <f t="shared" ref="M3:M17" si="1">E3*F3</f>
         <v>3.12</v>
       </c>
-      <c r="M3" s="9" t="s">
-        <v>85</v>
-      </c>
-      <c r="N3" s="11" t="s">
+      <c r="N3" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="O3" s="11" t="s">
         <v>87</v>
       </c>
-      <c r="O3" s="13" t="s">
+      <c r="P3" s="13" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:15" ht="36" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:16" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
         <v>7</v>
       </c>
@@ -985,21 +1013,24 @@
       <c r="I4" s="8"/>
       <c r="J4" s="8"/>
       <c r="K4" s="8"/>
-      <c r="L4" s="11">
+      <c r="L4" s="15">
+        <v>30</v>
+      </c>
+      <c r="M4" s="11">
         <f>E4*H4/10</f>
         <v>6.75</v>
       </c>
-      <c r="M4" s="9" t="s">
-        <v>85</v>
-      </c>
-      <c r="N4" s="11" t="s">
+      <c r="N4" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="O4" s="11" t="s">
         <v>88</v>
       </c>
-      <c r="O4" s="14" t="s">
+      <c r="P4" s="14" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:15" ht="36" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:16" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
         <v>16</v>
       </c>
@@ -1026,21 +1057,24 @@
       <c r="I5" s="8"/>
       <c r="J5" s="8"/>
       <c r="K5" s="8"/>
-      <c r="L5" s="11">
+      <c r="L5" s="15">
+        <v>4</v>
+      </c>
+      <c r="M5" s="11">
         <f t="shared" si="1"/>
         <v>1.24</v>
       </c>
-      <c r="M5" s="9" t="s">
-        <v>85</v>
-      </c>
-      <c r="N5" s="11" t="s">
+      <c r="N5" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="O5" s="11" t="s">
         <v>89</v>
       </c>
-      <c r="O5" s="13" t="s">
+      <c r="P5" s="13" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:15" ht="36" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:16" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
         <v>17</v>
       </c>
@@ -1067,21 +1101,24 @@
       <c r="I6" s="8"/>
       <c r="J6" s="8"/>
       <c r="K6" s="8"/>
-      <c r="L6" s="11">
+      <c r="L6" s="15">
+        <v>4</v>
+      </c>
+      <c r="M6" s="11">
         <f t="shared" si="1"/>
         <v>1.04</v>
       </c>
-      <c r="M6" s="9" t="s">
-        <v>85</v>
-      </c>
-      <c r="N6" s="11" t="s">
+      <c r="N6" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="O6" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="O6" s="13" t="s">
+      <c r="P6" s="13" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:15" ht="36" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:16" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
         <v>20</v>
       </c>
@@ -1108,21 +1145,24 @@
       <c r="I7" s="8"/>
       <c r="J7" s="8"/>
       <c r="K7" s="8"/>
-      <c r="L7" s="11">
+      <c r="L7" s="15">
+        <v>20</v>
+      </c>
+      <c r="M7" s="11">
         <f>(E7*H7)/10</f>
         <v>4.7</v>
       </c>
-      <c r="M7" s="9" t="s">
-        <v>85</v>
-      </c>
-      <c r="N7" s="11" t="s">
+      <c r="N7" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="O7" s="11" t="s">
         <v>91</v>
       </c>
-      <c r="O7" s="13" t="s">
+      <c r="P7" s="13" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:15" ht="36" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:16" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
         <v>23</v>
       </c>
@@ -1149,21 +1189,24 @@
       <c r="I8" s="8"/>
       <c r="J8" s="8"/>
       <c r="K8" s="8"/>
-      <c r="L8" s="11">
+      <c r="L8" s="15">
+        <v>4</v>
+      </c>
+      <c r="M8" s="11">
         <f t="shared" si="1"/>
         <v>23.44</v>
       </c>
-      <c r="M8" s="9" t="s">
-        <v>85</v>
-      </c>
-      <c r="N8" s="11" t="s">
+      <c r="N8" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="O8" s="11" t="s">
         <v>92</v>
       </c>
-      <c r="O8" s="13" t="s">
+      <c r="P8" s="13" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:15" ht="36" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:16" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
         <v>26</v>
       </c>
@@ -1190,21 +1233,24 @@
       <c r="I9" s="8"/>
       <c r="J9" s="8"/>
       <c r="K9" s="8"/>
-      <c r="L9" s="11">
+      <c r="L9" s="15">
+        <v>4</v>
+      </c>
+      <c r="M9" s="11">
         <f t="shared" si="1"/>
         <v>10.64</v>
       </c>
-      <c r="M9" s="9" t="s">
-        <v>85</v>
-      </c>
-      <c r="N9" s="11" t="s">
+      <c r="N9" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="O9" s="11" t="s">
         <v>93</v>
       </c>
-      <c r="O9" s="13" t="s">
+      <c r="P9" s="13" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="1:15" ht="36" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:16" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="s">
         <v>29</v>
       </c>
@@ -1231,21 +1277,24 @@
       <c r="I10" s="8"/>
       <c r="J10" s="8"/>
       <c r="K10" s="8"/>
-      <c r="L10" s="11">
+      <c r="L10" s="15">
+        <v>4</v>
+      </c>
+      <c r="M10" s="11">
         <f t="shared" si="1"/>
         <v>4.5599999999999996</v>
       </c>
-      <c r="M10" s="9" t="s">
-        <v>85</v>
-      </c>
-      <c r="N10" s="11" t="s">
+      <c r="N10" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="O10" s="11" t="s">
         <v>111</v>
       </c>
-      <c r="O10" s="14" t="s">
+      <c r="P10" s="14" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="11" spans="1:15" ht="36" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:16" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="s">
         <v>30</v>
       </c>
@@ -1272,21 +1321,24 @@
       </c>
       <c r="J11" s="8"/>
       <c r="K11" s="8"/>
-      <c r="L11" s="11">
+      <c r="L11" s="15">
+        <v>4</v>
+      </c>
+      <c r="M11" s="11">
         <f t="shared" si="1"/>
         <v>20.96</v>
       </c>
-      <c r="M11" s="9" t="s">
-        <v>85</v>
-      </c>
-      <c r="N11" s="11" t="s">
+      <c r="N11" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="O11" s="11" t="s">
         <v>96</v>
       </c>
-      <c r="O11" s="13" t="s">
+      <c r="P11" s="13" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="12" spans="1:15" ht="36" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:16" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="s">
         <v>33</v>
       </c>
@@ -1313,21 +1365,24 @@
       <c r="I12" s="8"/>
       <c r="J12" s="8"/>
       <c r="K12" s="8"/>
-      <c r="L12" s="11">
+      <c r="L12" s="15">
+        <v>4</v>
+      </c>
+      <c r="M12" s="11">
         <f t="shared" si="1"/>
         <v>1.4</v>
       </c>
-      <c r="M12" s="9" t="s">
-        <v>85</v>
-      </c>
-      <c r="N12" s="11" t="s">
+      <c r="N12" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="O12" s="11" t="s">
         <v>97</v>
       </c>
-      <c r="O12" s="13" t="s">
+      <c r="P12" s="13" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="13" spans="1:15" ht="36" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:16" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="7" t="s">
         <v>34</v>
       </c>
@@ -1354,21 +1409,24 @@
       <c r="I13" s="8"/>
       <c r="J13" s="8"/>
       <c r="K13" s="8"/>
-      <c r="L13" s="11">
+      <c r="L13" s="15">
+        <v>4</v>
+      </c>
+      <c r="M13" s="11">
         <f t="shared" si="1"/>
         <v>0.56000000000000005</v>
       </c>
-      <c r="M13" s="9" t="s">
-        <v>85</v>
-      </c>
-      <c r="N13" s="11" t="s">
+      <c r="N13" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="O13" s="11" t="s">
         <v>94</v>
       </c>
-      <c r="O13" s="13" t="s">
+      <c r="P13" s="13" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="14" spans="1:15" ht="36" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:16" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="7" t="s">
         <v>38</v>
       </c>
@@ -1395,21 +1453,24 @@
       <c r="I14" s="8"/>
       <c r="J14" s="8"/>
       <c r="K14" s="8"/>
-      <c r="L14" s="11">
+      <c r="L14" s="15">
+        <v>4</v>
+      </c>
+      <c r="M14" s="11">
         <f t="shared" si="1"/>
         <v>2.3199999999999998</v>
       </c>
-      <c r="M14" s="9" t="s">
-        <v>85</v>
-      </c>
-      <c r="N14" s="11" t="s">
+      <c r="N14" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="O14" s="11" t="s">
         <v>95</v>
       </c>
-      <c r="O14" s="13" t="s">
+      <c r="P14" s="13" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="15" spans="1:15" ht="36" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:16" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="7" t="s">
         <v>41</v>
       </c>
@@ -1436,21 +1497,24 @@
       <c r="I15" s="8"/>
       <c r="J15" s="8"/>
       <c r="K15" s="8"/>
-      <c r="L15" s="11">
+      <c r="L15" s="15">
+        <v>10</v>
+      </c>
+      <c r="M15" s="11">
         <f>E15*H15/10</f>
         <v>5.48</v>
       </c>
-      <c r="M15" s="9" t="s">
-        <v>85</v>
-      </c>
-      <c r="N15" s="11" t="s">
+      <c r="N15" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="O15" s="11" t="s">
         <v>98</v>
       </c>
-      <c r="O15" s="13" t="s">
+      <c r="P15" s="13" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="16" spans="1:15" ht="36" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:16" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="7" t="s">
         <v>43</v>
       </c>
@@ -1477,21 +1541,24 @@
       <c r="I16" s="8"/>
       <c r="J16" s="8"/>
       <c r="K16" s="8"/>
-      <c r="L16" s="11">
+      <c r="L16" s="15">
+        <v>4</v>
+      </c>
+      <c r="M16" s="11">
         <f t="shared" si="1"/>
         <v>7.44</v>
       </c>
-      <c r="M16" s="9" t="s">
-        <v>85</v>
-      </c>
-      <c r="N16" s="11" t="s">
+      <c r="N16" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="O16" s="11" t="s">
         <v>99</v>
       </c>
-      <c r="O16" s="13" t="s">
+      <c r="P16" s="13" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="17" spans="1:15" ht="36" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:16" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="7" t="s">
         <v>49</v>
       </c>
@@ -1518,21 +1585,24 @@
       <c r="I17" s="8"/>
       <c r="J17" s="8"/>
       <c r="K17" s="8"/>
-      <c r="L17" s="11">
+      <c r="L17" s="15">
+        <v>4</v>
+      </c>
+      <c r="M17" s="11">
         <f t="shared" si="1"/>
         <v>2.48</v>
       </c>
-      <c r="M17" s="9" t="s">
-        <v>85</v>
-      </c>
-      <c r="N17" s="11" t="s">
+      <c r="N17" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="O17" s="11" t="s">
         <v>100</v>
       </c>
-      <c r="O17" s="13" t="s">
+      <c r="P17" s="13" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="18" spans="1:15" ht="36" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:16" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="7" t="s">
         <v>53</v>
       </c>
@@ -1559,21 +1629,24 @@
       <c r="I18" s="8"/>
       <c r="J18" s="8"/>
       <c r="K18" s="8"/>
-      <c r="L18" s="11">
+      <c r="L18" s="15">
+        <v>10</v>
+      </c>
+      <c r="M18" s="11">
         <f>E18*H18/10</f>
         <v>1.41</v>
       </c>
-      <c r="M18" s="9" t="s">
-        <v>85</v>
-      </c>
-      <c r="N18" s="11" t="s">
+      <c r="N18" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="O18" s="11" t="s">
         <v>101</v>
       </c>
-      <c r="O18" s="13" t="s">
+      <c r="P18" s="13" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="19" spans="1:15" ht="36" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:16" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="7" t="s">
         <v>59</v>
       </c>
@@ -1602,21 +1675,24 @@
       <c r="K19" s="8">
         <v>0.8</v>
       </c>
-      <c r="L19" s="11">
+      <c r="L19" s="15">
+        <v>100</v>
+      </c>
+      <c r="M19" s="11">
         <f>E19*K19/100</f>
         <v>0.8</v>
       </c>
-      <c r="M19" s="9" t="s">
-        <v>85</v>
-      </c>
-      <c r="N19" s="11" t="s">
+      <c r="N19" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="O19" s="11" t="s">
         <v>102</v>
       </c>
-      <c r="O19" s="13" t="s">
+      <c r="P19" s="13" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="20" spans="1:15" ht="36" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:16" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="7" t="s">
         <v>62</v>
       </c>
@@ -1645,21 +1721,24 @@
       <c r="K20" s="8">
         <v>0.8</v>
       </c>
-      <c r="L20" s="11">
+      <c r="L20" s="15">
+        <v>100</v>
+      </c>
+      <c r="M20" s="11">
         <f>E20*K20/100</f>
         <v>0.8</v>
       </c>
-      <c r="M20" s="9" t="s">
-        <v>85</v>
-      </c>
-      <c r="N20" s="11" t="s">
+      <c r="N20" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="O20" s="11" t="s">
         <v>103</v>
       </c>
-      <c r="O20" s="13" t="s">
+      <c r="P20" s="13" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="21" spans="1:15" ht="36" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:16" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="7" t="s">
         <v>65</v>
       </c>
@@ -1686,21 +1765,24 @@
       <c r="I21" s="8"/>
       <c r="J21" s="8"/>
       <c r="K21" s="8"/>
-      <c r="L21" s="11">
+      <c r="L21" s="15">
+        <v>10</v>
+      </c>
+      <c r="M21" s="11">
         <f>E21*H21/10</f>
         <v>0.17</v>
       </c>
-      <c r="M21" s="9" t="s">
-        <v>85</v>
-      </c>
-      <c r="N21" s="11" t="s">
+      <c r="N21" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="O21" s="11" t="s">
         <v>104</v>
       </c>
-      <c r="O21" s="13" t="s">
+      <c r="P21" s="13" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="22" spans="1:15" ht="36" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:16" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="7" t="s">
         <v>68</v>
       </c>
@@ -1729,21 +1811,24 @@
       <c r="K22" s="8">
         <v>1.1000000000000001</v>
       </c>
-      <c r="L22" s="11">
+      <c r="L22" s="15">
+        <v>20</v>
+      </c>
+      <c r="M22" s="11">
         <f>E22*H22/10</f>
         <v>0.4</v>
       </c>
-      <c r="M22" s="9" t="s">
-        <v>85</v>
-      </c>
-      <c r="N22" s="11" t="s">
+      <c r="N22" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="O22" s="11" t="s">
         <v>105</v>
       </c>
-      <c r="O22" s="14" t="s">
+      <c r="P22" s="14" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="23" spans="1:15" ht="36" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:16" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="7" t="s">
         <v>51</v>
       </c>
@@ -1772,21 +1857,24 @@
       <c r="K23" s="8">
         <v>2.9</v>
       </c>
-      <c r="L23" s="11">
+      <c r="L23" s="16" t="s">
+        <v>113</v>
+      </c>
+      <c r="M23" s="11">
         <f>E23*K23/100</f>
         <v>2.9</v>
       </c>
-      <c r="M23" s="9" t="s">
-        <v>85</v>
-      </c>
-      <c r="N23" s="11" t="s">
+      <c r="N23" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="O23" s="11" t="s">
         <v>106</v>
       </c>
-      <c r="O23" s="13" t="s">
+      <c r="P23" s="13" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="24" spans="1:15" ht="36" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:16" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="7" t="s">
         <v>52</v>
       </c>
@@ -1815,21 +1903,24 @@
       <c r="K24" s="8">
         <v>6.7</v>
       </c>
-      <c r="L24" s="11">
+      <c r="L24" s="15">
+        <v>20</v>
+      </c>
+      <c r="M24" s="11">
         <f>E24*H24/10</f>
         <v>2</v>
       </c>
-      <c r="M24" s="9" t="s">
-        <v>85</v>
-      </c>
-      <c r="N24" s="11" t="s">
+      <c r="N24" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="O24" s="11" t="s">
         <v>107</v>
       </c>
-      <c r="O24" s="13" t="s">
+      <c r="P24" s="13" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="25" spans="1:15" ht="36" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:16" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="7" t="s">
         <v>76</v>
       </c>
@@ -1858,62 +1949,65 @@
       <c r="K25" s="8">
         <v>3.8</v>
       </c>
-      <c r="L25" s="11">
+      <c r="L25" s="16" t="s">
+        <v>113</v>
+      </c>
+      <c r="M25" s="11">
         <f>E25*H25/10</f>
         <v>4.4399999999999995</v>
       </c>
-      <c r="M25" s="9" t="s">
-        <v>85</v>
-      </c>
-      <c r="N25" s="11" t="s">
+      <c r="N25" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="O25" s="11" t="s">
         <v>108</v>
       </c>
-      <c r="O25" s="13" t="s">
+      <c r="P25" s="13" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="26" spans="1:15" ht="36" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="L26" s="12">
-        <f>SUM(L2:L25)</f>
+    <row r="26" spans="1:16" ht="36" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="M26" s="12">
+        <f>SUM(M2:M25)</f>
         <v>126.57000000000001</v>
       </c>
-      <c r="M26" s="5"/>
       <c r="N26" s="5"/>
-    </row>
-    <row r="27" spans="1:15" ht="36" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="N27" s="10"/>
+      <c r="O26" s="5"/>
+    </row>
+    <row r="27" spans="1:16" ht="36" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="O27" s="10"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="O2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="O3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="O4" r:id="rId3" xr:uid="{2485A731-BEBD-4A8A-9A5B-72A220997EEE}"/>
-    <hyperlink ref="O5" r:id="rId4" xr:uid="{3257BE96-96C8-4FFD-9FA0-19258A698561}"/>
-    <hyperlink ref="O6" r:id="rId5" xr:uid="{A9AA0BD4-CD63-446A-8A68-5E5E88F7958E}"/>
-    <hyperlink ref="O7" r:id="rId6" xr:uid="{55B193BF-2E90-4498-B29C-3DAC9AB29B48}"/>
-    <hyperlink ref="O8" r:id="rId7" xr:uid="{2330A808-ACC7-4028-948D-F112A01E3F7C}"/>
-    <hyperlink ref="O9" r:id="rId8" xr:uid="{2E676BDC-F980-463C-AD06-DCC59EE13105}"/>
-    <hyperlink ref="O11" r:id="rId9" xr:uid="{77A12C3E-331B-49E3-A8C7-36B37D7DD192}"/>
-    <hyperlink ref="O12" r:id="rId10" xr:uid="{C32F3B22-A079-4E56-B174-9EBE03836C72}"/>
-    <hyperlink ref="O13" r:id="rId11" xr:uid="{E52E5EF6-21E8-400A-AF4E-9F29D668C0FD}"/>
-    <hyperlink ref="O14" r:id="rId12" xr:uid="{77DFA638-23E7-47C2-AD09-D6D863331255}"/>
-    <hyperlink ref="O15" r:id="rId13" xr:uid="{C9F56E4E-1E61-4952-AFCF-891F096F7A72}"/>
-    <hyperlink ref="O16" r:id="rId14" xr:uid="{5DD4FAE6-2FD1-4EC6-BDBF-9B32386CFDC5}"/>
-    <hyperlink ref="O17" r:id="rId15" xr:uid="{FCC26BD1-AC90-4ABC-AC09-010AD9C4219F}"/>
-    <hyperlink ref="O18" r:id="rId16" xr:uid="{2B49BA75-63C8-45AD-A2D2-016FC9231156}"/>
-    <hyperlink ref="O19" r:id="rId17" xr:uid="{102FFB0F-0C49-4F42-AEC1-1D8B81F916D1}"/>
-    <hyperlink ref="O20" r:id="rId18" xr:uid="{8A6332C7-2C9E-426D-B47E-A4C4EA1330F2}"/>
-    <hyperlink ref="O21" r:id="rId19" xr:uid="{0ED1CEFE-1D0A-43F8-80BE-D6B83FF8DB73}"/>
-    <hyperlink ref="O23" r:id="rId20" xr:uid="{AC1CB978-EF99-43DD-BF4A-1C75C476F601}"/>
-    <hyperlink ref="O24" r:id="rId21" xr:uid="{D9EA7F5A-6248-471C-BFD2-D0594D713B6A}"/>
-    <hyperlink ref="O25" r:id="rId22" xr:uid="{F2E7AE5F-A921-4FAB-BE69-C0571DC19715}"/>
-    <hyperlink ref="O22" r:id="rId23" xr:uid="{6E402AD8-CC21-4FE9-80A8-DCBBC32369FB}"/>
-    <hyperlink ref="O10" r:id="rId24" xr:uid="{1DA94635-DA6F-4444-B2E8-79CE1ADC0ADB}"/>
+    <hyperlink ref="P2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="P3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="P4" r:id="rId3" xr:uid="{2485A731-BEBD-4A8A-9A5B-72A220997EEE}"/>
+    <hyperlink ref="P5" r:id="rId4" xr:uid="{3257BE96-96C8-4FFD-9FA0-19258A698561}"/>
+    <hyperlink ref="P6" r:id="rId5" xr:uid="{A9AA0BD4-CD63-446A-8A68-5E5E88F7958E}"/>
+    <hyperlink ref="P7" r:id="rId6" xr:uid="{55B193BF-2E90-4498-B29C-3DAC9AB29B48}"/>
+    <hyperlink ref="P8" r:id="rId7" xr:uid="{2330A808-ACC7-4028-948D-F112A01E3F7C}"/>
+    <hyperlink ref="P9" r:id="rId8" xr:uid="{2E676BDC-F980-463C-AD06-DCC59EE13105}"/>
+    <hyperlink ref="P11" r:id="rId9" xr:uid="{77A12C3E-331B-49E3-A8C7-36B37D7DD192}"/>
+    <hyperlink ref="P12" r:id="rId10" xr:uid="{C32F3B22-A079-4E56-B174-9EBE03836C72}"/>
+    <hyperlink ref="P13" r:id="rId11" xr:uid="{E52E5EF6-21E8-400A-AF4E-9F29D668C0FD}"/>
+    <hyperlink ref="P14" r:id="rId12" xr:uid="{77DFA638-23E7-47C2-AD09-D6D863331255}"/>
+    <hyperlink ref="P15" r:id="rId13" xr:uid="{C9F56E4E-1E61-4952-AFCF-891F096F7A72}"/>
+    <hyperlink ref="P16" r:id="rId14" xr:uid="{5DD4FAE6-2FD1-4EC6-BDBF-9B32386CFDC5}"/>
+    <hyperlink ref="P17" r:id="rId15" xr:uid="{FCC26BD1-AC90-4ABC-AC09-010AD9C4219F}"/>
+    <hyperlink ref="P18" r:id="rId16" xr:uid="{2B49BA75-63C8-45AD-A2D2-016FC9231156}"/>
+    <hyperlink ref="P19" r:id="rId17" xr:uid="{102FFB0F-0C49-4F42-AEC1-1D8B81F916D1}"/>
+    <hyperlink ref="P20" r:id="rId18" xr:uid="{8A6332C7-2C9E-426D-B47E-A4C4EA1330F2}"/>
+    <hyperlink ref="P21" r:id="rId19" xr:uid="{0ED1CEFE-1D0A-43F8-80BE-D6B83FF8DB73}"/>
+    <hyperlink ref="P23" r:id="rId20" xr:uid="{AC1CB978-EF99-43DD-BF4A-1C75C476F601}"/>
+    <hyperlink ref="P24" r:id="rId21" xr:uid="{D9EA7F5A-6248-471C-BFD2-D0594D713B6A}"/>
+    <hyperlink ref="P25" r:id="rId22" xr:uid="{F2E7AE5F-A921-4FAB-BE69-C0571DC19715}"/>
+    <hyperlink ref="P22" r:id="rId23" xr:uid="{6E402AD8-CC21-4FE9-80A8-DCBBC32369FB}"/>
+    <hyperlink ref="P10" r:id="rId24" xr:uid="{1DA94635-DA6F-4444-B2E8-79CE1ADC0ADB}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId25"/>
   <ignoredErrors>
-    <ignoredError sqref="L4 L7 L15 L23" formula="1"/>
+    <ignoredError sqref="M4 M7 M15 M23" formula="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>